<commit_message>
Update Tax Rate % in some models for uniformity
</commit_message>
<xml_diff>
--- a/$NKE.xlsx
+++ b/$NKE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9CB87B-41A6-4882-AC3E-00C9C5853C74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C6CEE2-B065-4356-A13C-87D1B67C02C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="495" windowWidth="31095" windowHeight="18900" xr2:uid="{7612E5BF-E27D-45C9-936D-073FAE02F148}"/>
+    <workbookView xWindow="2505" yWindow="495" windowWidth="31095" windowHeight="18900" activeTab="1" xr2:uid="{7612E5BF-E27D-45C9-936D-073FAE02F148}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -289,9 +289,6 @@
     <t>Net Margin</t>
   </si>
   <si>
-    <t>Taxes %</t>
-  </si>
-  <si>
     <t>Balance Sheet</t>
   </si>
   <si>
@@ -449,6 +446,9 @@
   </si>
   <si>
     <t>Inventory/Revenue</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
   </si>
 </sst>
 </file>
@@ -780,10 +780,33 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -796,29 +819,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1309,7 +1309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EA867B-521D-45A9-9B00-27085D6F4DA0}">
   <dimension ref="A2:V40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C27" sqref="C27:D27"/>
     </sheetView>
   </sheetViews>
@@ -1332,16 +1332,16 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-      <c r="T5" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="U5" s="61"/>
-      <c r="V5" s="62"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="T5" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="U5" s="58"/>
+      <c r="V5" s="59"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -1352,7 +1352,7 @@
       </c>
       <c r="D6" s="39"/>
       <c r="T6" s="43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="U6" s="7"/>
       <c r="V6" s="8"/>
@@ -1368,7 +1368,7 @@
         <v>68</v>
       </c>
       <c r="T7" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U7" s="7"/>
       <c r="V7" s="8"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="D8" s="39"/>
       <c r="T8" s="42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U8" s="7"/>
       <c r="V8" s="8"/>
@@ -1400,7 +1400,7 @@
         <v>68</v>
       </c>
       <c r="T9" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="8"/>
@@ -1417,7 +1417,7 @@
         <v>68</v>
       </c>
       <c r="T10" s="42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U10" s="7"/>
       <c r="V10" s="8"/>
@@ -1434,7 +1434,7 @@
         <v>68</v>
       </c>
       <c r="T11" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U11" s="7"/>
       <c r="V11" s="8"/>
@@ -1449,17 +1449,17 @@
       </c>
       <c r="D12" s="40"/>
       <c r="T12" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U12" s="9"/>
       <c r="V12" s="10"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1468,10 +1468,10 @@
       <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="55"/>
+      <c r="D16" s="61"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -1480,10 +1480,10 @@
       <c r="B17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="61"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
@@ -1492,66 +1492,66 @@
       <c r="B18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="55"/>
+      <c r="D18" s="61"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="59"/>
+      <c r="D19" s="68"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="62"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="59"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="55"/>
+      <c r="D23" s="61"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="54">
+      <c r="C24" s="60">
         <v>1964</v>
       </c>
-      <c r="D24" s="55"/>
+      <c r="D24" s="61"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="65"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="63"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="67">
+      <c r="C26" s="64">
         <f>'Financial Model'!W44</f>
         <v>9662</v>
       </c>
-      <c r="D26" s="55"/>
+      <c r="D26" s="61"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="11"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="66"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="63"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="11" t="s">
@@ -1560,7 +1560,7 @@
       <c r="C28" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="68">
+      <c r="D28" s="54">
         <v>44833</v>
       </c>
     </row>
@@ -1568,94 +1568,86 @@
       <c r="B29" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="64"/>
+      <c r="D29" s="56"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="59"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C33" s="56">
+        <v>126</v>
+      </c>
+      <c r="C33" s="65">
         <f>C12/('Financial Model'!AD21*1000)</f>
         <v>24.304770592127053</v>
       </c>
-      <c r="D33" s="57"/>
+      <c r="D33" s="66"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C34" s="56">
+        <v>127</v>
+      </c>
+      <c r="C34" s="65">
         <f>C6/('Financial Model'!AD22*1000)</f>
         <v>24.880641209063874</v>
       </c>
-      <c r="D34" s="57"/>
+      <c r="D34" s="66"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="55"/>
+        <v>128</v>
+      </c>
+      <c r="C35" s="60"/>
+      <c r="D35" s="61"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="56">
+        <v>129</v>
+      </c>
+      <c r="C36" s="65">
         <f>C6/'Financial Model'!W70</f>
         <v>9.4420201618000252</v>
       </c>
-      <c r="D36" s="57"/>
+      <c r="D36" s="66"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="11"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="55"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="61"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" s="56">
+        <v>130</v>
+      </c>
+      <c r="C38" s="65">
         <f>'Financial Model'!AC79/('Financial Model'!AC22*1000)</f>
         <v>37.504159682207103</v>
       </c>
-      <c r="D38" s="57"/>
+      <c r="D38" s="66"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C39" s="54"/>
-      <c r="D39" s="55"/>
+        <v>131</v>
+      </c>
+      <c r="C39" s="60"/>
+      <c r="D39" s="61"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="59"/>
+        <v>132</v>
+      </c>
+      <c r="C40" s="67"/>
+      <c r="D40" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
@@ -1671,6 +1663,14 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{6430964A-0169-5B4A-BCFC-F02355D9307D}"/>
@@ -1685,11 +1685,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F137E7D-55F8-4ACC-BDF9-DCDC53EC521C}">
   <dimension ref="A1:AO85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q30" sqref="Q30"/>
+      <selection pane="bottomRight" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1705,7 +1705,7 @@
   <sheetData>
     <row r="1" spans="1:41" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>48</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="3" spans="1:41" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G3" s="29">
         <v>6.0359999999999996</v>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="4" spans="1:41" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" s="29">
         <v>2.9489999999999998</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="5" spans="1:41" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" s="29">
         <v>0.41599999999999998</v>
@@ -2103,7 +2103,7 @@
     </row>
     <row r="6" spans="1:41" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="29">
         <v>1.6E-2</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="7" spans="1:41" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" s="27">
         <f t="shared" ref="G7:W7" si="2">SUM(G3:G6)</f>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="8" spans="1:41" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G8" s="27">
         <v>0.52700000000000002</v>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="9" spans="1:41" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G9" s="27">
         <v>4.0000000000000001E-3</v>
@@ -3538,16 +3538,16 @@
         <v>82</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K25" s="21">
         <f t="shared" ref="K25" si="21">K10/G10-1</f>
@@ -3602,10 +3602,10 @@
         <v>3.5842586544742483E-2</v>
       </c>
       <c r="Z25" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA25" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB25" s="21">
         <f t="shared" ref="AB25" si="27">AB10/AA10-1</f>
@@ -3622,19 +3622,19 @@
     </row>
     <row r="26" spans="2:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K26" s="34">
         <f t="shared" ref="K26:K28" si="29">K3/G3-1</f>
@@ -3689,10 +3689,10 @@
         <v>5.1308629178543841E-2</v>
       </c>
       <c r="Z26" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA26" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB26" s="34">
         <f t="shared" ref="AB26" si="35">AB3/AA3-1</f>
@@ -3709,19 +3709,19 @@
     </row>
     <row r="27" spans="2:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K27" s="34">
         <f t="shared" si="29"/>
@@ -3776,10 +3776,10 @@
         <v>-4.6376811594203149E-3</v>
       </c>
       <c r="Z27" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA27" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB27" s="34">
         <f t="shared" ref="AB27" si="38">AB4/AA4-1</f>
@@ -3796,19 +3796,19 @@
     </row>
     <row r="28" spans="2:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K28" s="34">
         <f t="shared" si="29"/>
@@ -3863,10 +3863,10 @@
         <v>4.5161290322580649E-2</v>
       </c>
       <c r="Z28" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB28" s="34">
         <f t="shared" ref="AB28" si="40">AB5/AA5-1</f>
@@ -3883,19 +3883,19 @@
     </row>
     <row r="29" spans="2:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K29" s="34">
         <f t="shared" ref="K29:K31" si="42">K7/G7-1</f>
@@ -3950,10 +3950,10 @@
         <v>3.5051546391752897E-2</v>
       </c>
       <c r="Z29" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA29" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB29" s="34">
         <f t="shared" ref="AB29" si="49">AB7/AA7-1</f>
@@ -3970,19 +3970,19 @@
     </row>
     <row r="30" spans="2:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H30" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K30" s="34">
         <f t="shared" si="42"/>
@@ -4037,10 +4037,10 @@
         <v>2.2257551669316422E-2</v>
       </c>
       <c r="Z30" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA30" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB30" s="34">
         <f t="shared" ref="AB30" si="51">AB8/AA8-1</f>
@@ -4057,19 +4057,19 @@
     </row>
     <row r="31" spans="2:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K31" s="34">
         <f t="shared" si="42"/>
@@ -4080,7 +4080,7 @@
         <v>-0.33333333333333337</v>
       </c>
       <c r="M31" s="49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N31" s="34">
         <f t="shared" si="43"/>
@@ -4123,10 +4123,10 @@
         <v>-0.80952380952380953</v>
       </c>
       <c r="Z31" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA31" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB31" s="34">
         <f t="shared" ref="AB31" si="53">AB9/AA9-1</f>
@@ -4146,7 +4146,7 @@
         <v>83</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H32" s="25">
         <f t="shared" ref="H32:L32" si="54">H10/G10-1</f>
@@ -4213,13 +4213,13 @@
         <v>3.7027954879843117E-2</v>
       </c>
       <c r="Z32" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA32" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AD32" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.2">
@@ -4491,7 +4491,7 @@
     </row>
     <row r="37" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G37" s="25">
         <f t="shared" ref="G37" si="92">G20/G19</f>
@@ -4580,7 +4580,7 @@
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B40" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="2:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4649,7 +4649,7 @@
     </row>
     <row r="42" spans="2:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G42" s="19">
         <v>987</v>
@@ -4713,7 +4713,7 @@
     </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G43" s="20">
         <v>4330</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="44" spans="2:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G44" s="19">
         <v>5227</v>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="45" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G45" s="20">
         <v>1675</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="46" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G46" s="20">
         <f t="shared" ref="G46:L46" si="105">SUM(G41:G45)</f>
@@ -4986,7 +4986,7 @@
     </row>
     <row r="47" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G47" s="20">
         <v>4487</v>
@@ -5050,7 +5050,7 @@
     </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G48" s="20">
         <v>0</v>
@@ -5114,7 +5114,7 @@
     </row>
     <row r="49" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G49" s="20">
         <f>284+154</f>
@@ -5195,7 +5195,7 @@
     </row>
     <row r="50" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G50" s="20">
         <v>2057</v>
@@ -5259,7 +5259,7 @@
     </row>
     <row r="51" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G51" s="20">
         <f t="shared" ref="G51:L51" si="108">G46+SUM(G47:G50)</f>
@@ -5359,7 +5359,7 @@
     </row>
     <row r="53" spans="2:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G53" s="19">
         <v>6</v>
@@ -5423,7 +5423,7 @@
     </row>
     <row r="54" spans="2:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G54" s="19">
         <v>13</v>
@@ -5487,7 +5487,7 @@
     </row>
     <row r="55" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G55" s="20">
         <v>2333</v>
@@ -5551,7 +5551,7 @@
     </row>
     <row r="56" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G56" s="20">
         <v>0</v>
@@ -5615,7 +5615,7 @@
     </row>
     <row r="57" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G57" s="20">
         <v>4174</v>
@@ -5679,7 +5679,7 @@
     </row>
     <row r="58" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G58" s="20">
         <v>182</v>
@@ -5743,7 +5743,7 @@
     </row>
     <row r="59" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G59" s="20">
         <f t="shared" ref="G59:L59" si="113">SUM(G53:G58)</f>
@@ -5824,7 +5824,7 @@
     </row>
     <row r="60" spans="2:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G60" s="19">
         <v>3467</v>
@@ -5888,7 +5888,7 @@
     </row>
     <row r="61" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G61" s="20">
         <v>0</v>
@@ -5952,7 +5952,7 @@
     </row>
     <row r="62" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G62" s="20">
         <v>3316</v>
@@ -6016,7 +6016,7 @@
     </row>
     <row r="63" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G63" s="20">
         <v>0</v>
@@ -6080,7 +6080,7 @@
     </row>
     <row r="64" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G64" s="20">
         <f t="shared" ref="G64:L64" si="117">G59+SUM(G60:G63)</f>
@@ -6178,7 +6178,7 @@
     </row>
     <row r="66" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G66" s="20">
         <v>8992</v>
@@ -6241,7 +6241,7 @@
     </row>
     <row r="67" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G67" s="20">
         <f t="shared" ref="G67:W67" si="119">G66+G64</f>
@@ -6338,7 +6338,7 @@
     </row>
     <row r="69" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G69" s="20">
         <f t="shared" ref="G69:V69" si="120">G51-G64</f>
@@ -6419,7 +6419,7 @@
     </row>
     <row r="70" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G70" s="20">
         <f t="shared" ref="G70:V70" si="122">G69/G23</f>
@@ -6500,19 +6500,19 @@
     </row>
     <row r="72" spans="2:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B72" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J72" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K72" s="34">
         <f>K44/G44-1</f>
@@ -6573,10 +6573,10 @@
     </row>
     <row r="73" spans="2:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B73" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H73" s="34">
         <f t="shared" ref="H73:V73" si="127">H44/G44-1</f>
@@ -6643,7 +6643,7 @@
         <v>0.14750593824228031</v>
       </c>
       <c r="AD73" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="2:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -6894,7 +6894,7 @@
     </row>
     <row r="79" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G79" s="1">
         <v>82.2</v>
@@ -6958,7 +6958,7 @@
     </row>
     <row r="80" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G80" s="20">
         <f>G79*G23</f>
@@ -7120,7 +7120,7 @@
     </row>
     <row r="83" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AA83" s="52"/>
       <c r="AB83" s="52"/>
@@ -7135,7 +7135,7 @@
     </row>
     <row r="85" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G85" s="25">
         <f t="shared" ref="G85:W85" si="159">G44/(G10*1000)</f>

</xml_diff>

<commit_message>
Misc updates to fashion models
</commit_message>
<xml_diff>
--- a/$NKE.xlsx
+++ b/$NKE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C6CEE2-B065-4356-A13C-87D1B67C02C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4964CFCC-83BF-49AF-A691-848DBB83B055}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="495" windowWidth="31095" windowHeight="18900" activeTab="1" xr2:uid="{7612E5BF-E27D-45C9-936D-073FAE02F148}"/>
+    <workbookView xWindow="2505" yWindow="495" windowWidth="31095" windowHeight="18900" xr2:uid="{7612E5BF-E27D-45C9-936D-073FAE02F148}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="142">
   <si>
     <t>$NKE</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>Key Events</t>
   </si>
 </sst>
 </file>
@@ -679,7 +682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -783,30 +786,12 @@
     <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -821,6 +806,28 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1309,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EA867B-521D-45A9-9B00-27085D6F4DA0}">
   <dimension ref="A2:V40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:D27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1332,25 +1339,53 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="T5" s="57" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="65"/>
+      <c r="F5" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="65"/>
+      <c r="T5" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="58"/>
-      <c r="V5" s="59"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="65"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4">
-        <v>95.33</v>
+        <v>93.83</v>
       </c>
       <c r="D6" s="39"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55"/>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="56"/>
       <c r="T6" s="43" t="s">
         <v>134</v>
       </c>
@@ -1367,6 +1402,19 @@
       <c r="D7" s="39" t="s">
         <v>68</v>
       </c>
+      <c r="F7" s="71"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="55"/>
+      <c r="R7" s="56"/>
       <c r="T7" s="42" t="s">
         <v>89</v>
       </c>
@@ -1379,9 +1427,22 @@
       </c>
       <c r="C8" s="37">
         <f>C6*C7</f>
-        <v>149391.64299999998</v>
+        <v>147040.99299999999</v>
       </c>
       <c r="D8" s="39"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="56"/>
       <c r="T8" s="42" t="s">
         <v>88</v>
       </c>
@@ -1399,6 +1460,19 @@
       <c r="D9" s="39" t="s">
         <v>68</v>
       </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="56"/>
       <c r="T9" s="42" t="s">
         <v>90</v>
       </c>
@@ -1416,6 +1490,19 @@
       <c r="D10" s="39" t="s">
         <v>68</v>
       </c>
+      <c r="F10" s="71"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="56"/>
       <c r="T10" s="42" t="s">
         <v>91</v>
       </c>
@@ -1433,6 +1520,19 @@
       <c r="D11" s="39" t="s">
         <v>68</v>
       </c>
+      <c r="F11" s="71"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="56"/>
       <c r="T11" s="43" t="s">
         <v>93</v>
       </c>
@@ -1445,21 +1545,77 @@
       </c>
       <c r="C12" s="38">
         <f>C8-C11</f>
-        <v>146946.64299999998</v>
+        <v>144595.99299999999</v>
       </c>
       <c r="D12" s="40"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="55"/>
+      <c r="P12" s="55"/>
+      <c r="Q12" s="55"/>
+      <c r="R12" s="56"/>
       <c r="T12" s="44" t="s">
         <v>94</v>
       </c>
       <c r="U12" s="9"/>
       <c r="V12" s="10"/>
     </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="F13" s="71"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="55"/>
+      <c r="R13" s="56"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="F14" s="71"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="55"/>
+      <c r="P14" s="55"/>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="56"/>
+    </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="56"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1468,92 +1624,252 @@
       <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="61"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="58"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="56"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="61"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="58"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="56"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="61"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="58"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="56"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="68"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="57" t="s">
+      <c r="D19" s="62"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="56"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F20" s="71"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="56"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F21" s="71"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="56"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B22" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="59"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="56"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="61"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="58"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="56"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="60">
+      <c r="C24" s="57">
         <v>1964</v>
       </c>
-      <c r="D24" s="61"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="58"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="56"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C25" s="68"/>
+      <c r="D25" s="69"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="56"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="64">
+      <c r="C26" s="70">
         <f>'Financial Model'!W44</f>
         <v>9662</v>
       </c>
-      <c r="D26" s="61"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="58"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="56"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B27" s="11"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="63"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C27" s="68"/>
+      <c r="D27" s="69"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="55"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="55"/>
+      <c r="R27" s="56"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B28" s="11" t="s">
         <v>18</v>
       </c>
@@ -1563,91 +1879,272 @@
       <c r="D28" s="54">
         <v>44833</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F28" s="71"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="56"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B29" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="55" t="s">
+      <c r="C29" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="56"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="57" t="s">
+      <c r="D29" s="67"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="55"/>
+      <c r="R29" s="56"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F30" s="71"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="55"/>
+      <c r="P30" s="55"/>
+      <c r="Q30" s="55"/>
+      <c r="R30" s="56"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F31" s="71"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="55"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="55"/>
+      <c r="Q31" s="55"/>
+      <c r="R31" s="56"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B32" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="64"/>
+      <c r="D32" s="65"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="55"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="55"/>
+      <c r="Q32" s="55"/>
+      <c r="R32" s="56"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B33" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C33" s="65">
+      <c r="C33" s="59">
         <f>C12/('Financial Model'!AD21*1000)</f>
-        <v>24.304770592127053</v>
-      </c>
-      <c r="D33" s="66"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+        <v>23.915976347998704</v>
+      </c>
+      <c r="D33" s="60"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="55"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="55"/>
+      <c r="Q33" s="55"/>
+      <c r="R33" s="56"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C34" s="65">
+      <c r="C34" s="59">
         <f>C6/('Financial Model'!AD22*1000)</f>
-        <v>24.880641209063874</v>
-      </c>
-      <c r="D34" s="66"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+        <v>24.48914890009927</v>
+      </c>
+      <c r="D34" s="60"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="55"/>
+      <c r="N34" s="55"/>
+      <c r="O34" s="55"/>
+      <c r="P34" s="55"/>
+      <c r="Q34" s="55"/>
+      <c r="R34" s="56"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="61"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="56"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="65">
+      <c r="C36" s="59">
         <f>C6/'Financial Model'!W70</f>
-        <v>9.4420201618000252</v>
-      </c>
-      <c r="D36" s="66"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+        <v>9.2934517128049539</v>
+      </c>
+      <c r="D36" s="60"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="55"/>
+      <c r="R36" s="56"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B37" s="11"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="61"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C37" s="57"/>
+      <c r="D37" s="58"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="55"/>
+      <c r="M37" s="55"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="55"/>
+      <c r="P37" s="55"/>
+      <c r="Q37" s="55"/>
+      <c r="R37" s="56"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C38" s="65">
+      <c r="C38" s="59">
         <f>'Financial Model'!AC79/('Financial Model'!AC22*1000)</f>
         <v>37.504159682207103</v>
       </c>
-      <c r="D38" s="66"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="60"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="55"/>
+      <c r="N38" s="55"/>
+      <c r="O38" s="55"/>
+      <c r="P38" s="55"/>
+      <c r="Q38" s="55"/>
+      <c r="R38" s="56"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="60"/>
-      <c r="D39" s="61"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C39" s="57"/>
+      <c r="D39" s="58"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="55"/>
+      <c r="O39" s="55"/>
+      <c r="P39" s="55"/>
+      <c r="Q39" s="55"/>
+      <c r="R39" s="56"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B40" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C40" s="67"/>
-      <c r="D40" s="68"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="62"/>
+      <c r="F40" s="72"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="F5:R5"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
@@ -1664,13 +2161,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{6430964A-0169-5B4A-BCFC-F02355D9307D}"/>
@@ -1685,7 +2175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F137E7D-55F8-4ACC-BDF9-DCDC53EC521C}">
   <dimension ref="A1:AO85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>